<commit_message>
add dates to files
</commit_message>
<xml_diff>
--- a/_data/WePlayData/CleanedWPCIncomingParentReflection.xlsx
+++ b/_data/WePlayData/CleanedWPCIncomingParentReflection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renarepenning/Desktop/DS Project Sheets/WePLAYCenterSurveyData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renarepenning/Desktop/School/weplaynoladata/_data/WePlayData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1272BE-54BF-CF4A-A6AE-0641AC458D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0028A02C-61CD-9745-A0B0-5C3808C38B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6500" yWindow="460" windowWidth="20120" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="183">
   <si>
     <t>First Name</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>Grandparent</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -626,9 +629,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,115 +971,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ23"/>
+  <dimension ref="A1:CA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BJ23" sqref="BJ23"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:79" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="BX1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BZ1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:78" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:79" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>182</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
@@ -1084,22 +1091,22 @@
         <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>32</v>
@@ -1117,34 +1124,34 @@
         <v>32</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>32</v>
@@ -1156,151 +1163,151 @@
         <v>32</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BH2" s="1" t="s">
+      <c r="BI2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BI2" s="1" t="s">
+      <c r="BJ2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BK2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BK2" s="1" t="s">
+      <c r="BL2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BL2" s="1" t="s">
+      <c r="BM2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BN2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="BO2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="BP2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BT2" s="1" t="s">
+      <c r="BU2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BU2" s="1" t="s">
+      <c r="BV2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BV2" s="1" t="s">
+      <c r="BW2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="BW2" s="1" t="s">
+      <c r="BX2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="BX2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="BY2" s="1" t="s">
         <v>34</v>
@@ -1308,64 +1315,67 @@
       <c r="BZ2" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="CA2" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>43843</v>
+      </c>
+      <c r="B3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>83</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>70122</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>85</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>86</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>87</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>88</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>89</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>90</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>91</v>
       </c>
       <c r="AC3" t="s">
         <v>91</v>
       </c>
       <c r="AD3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AE3" t="s">
         <v>92</v>
       </c>
       <c r="AF3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AG3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AH3" t="s">
         <v>92</v>
@@ -1380,124 +1390,127 @@
         <v>92</v>
       </c>
       <c r="AL3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN3" t="s">
         <v>94</v>
       </c>
-      <c r="AN3" t="s">
-        <v>95</v>
-      </c>
       <c r="AO3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP3" t="s">
         <v>94</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>96</v>
       </c>
-      <c r="AQ3" t="s">
-        <v>97</v>
-      </c>
       <c r="AR3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AS3" t="s">
         <v>96</v>
       </c>
       <c r="AT3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AU3" t="s">
         <v>97</v>
       </c>
       <c r="AV3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AW3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX3" t="s">
         <v>94</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>96</v>
       </c>
       <c r="AY3" t="s">
         <v>96</v>
       </c>
       <c r="AZ3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA3" t="s">
         <v>90</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
         <v>98</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BD3" t="s">
         <v>64</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BF3" t="s">
         <v>66</v>
       </c>
-      <c r="BM3" t="s">
+      <c r="BN3" t="s">
         <v>99</v>
       </c>
-      <c r="BO3" t="s">
+      <c r="BP3" t="s">
         <v>75</v>
       </c>
-      <c r="BV3" t="s">
+      <c r="BW3" t="s">
         <v>100</v>
       </c>
-      <c r="BW3" t="s">
+      <c r="BX3" t="s">
         <v>101</v>
       </c>
-      <c r="BY3" t="s">
+      <c r="BZ3" t="s">
         <v>102</v>
       </c>
-      <c r="BZ3" t="s">
+      <c r="CA3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>43819</v>
+      </c>
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>84</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>104</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>70072</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>85</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>105</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>87</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>88</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>106</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>90</v>
       </c>
-      <c r="AB4" t="s">
-        <v>93</v>
-      </c>
       <c r="AC4" t="s">
         <v>93</v>
       </c>
@@ -1529,7 +1542,7 @@
         <v>93</v>
       </c>
       <c r="AM4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN4" t="s">
         <v>95</v>
@@ -1541,111 +1554,114 @@
         <v>95</v>
       </c>
       <c r="AQ4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AR4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS4" t="s">
         <v>96</v>
       </c>
-      <c r="AS4" t="s">
-        <v>97</v>
-      </c>
       <c r="AT4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AV4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AW4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX4" t="s">
         <v>94</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AY4" t="s">
         <v>96</v>
       </c>
-      <c r="AY4" t="s">
-        <v>95</v>
-      </c>
       <c r="AZ4" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA4" t="s">
         <v>90</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BC4" t="s">
         <v>63</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BE4" t="s">
         <v>65</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BF4" t="s">
         <v>66</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="BI4" t="s">
         <v>69</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="BP4" t="s">
         <v>75</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="BQ4" t="s">
         <v>76</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="BX4" t="s">
         <v>101</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="BZ4" t="s">
         <v>107</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CA4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>43817</v>
+      </c>
+      <c r="B5" t="s">
         <v>88</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>109</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>110</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>70119</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>111</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>112</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>113</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>88</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>90</v>
       </c>
-      <c r="AB5" t="s">
-        <v>93</v>
-      </c>
       <c r="AC5" t="s">
         <v>93</v>
       </c>
       <c r="AD5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AE5" t="s">
         <v>92</v>
@@ -1654,25 +1670,25 @@
         <v>92</v>
       </c>
       <c r="AG5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AH5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AI5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AJ5" t="s">
         <v>93</v>
       </c>
       <c r="AK5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AL5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN5" t="s">
         <v>95</v>
@@ -1687,13 +1703,13 @@
         <v>95</v>
       </c>
       <c r="AR5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS5" t="s">
         <v>94</v>
       </c>
-      <c r="AS5" t="s">
-        <v>97</v>
-      </c>
       <c r="AT5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU5" t="s">
         <v>95</v>
@@ -1702,85 +1718,88 @@
         <v>95</v>
       </c>
       <c r="AW5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX5" t="s">
         <v>94</v>
       </c>
-      <c r="AX5" t="s">
-        <v>97</v>
-      </c>
       <c r="AY5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AZ5" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA5" t="s">
         <v>101</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BB5" t="s">
         <v>115</v>
       </c>
-      <c r="BO5" t="s">
+      <c r="BP5" t="s">
         <v>75</v>
       </c>
-      <c r="BP5" t="s">
+      <c r="BQ5" t="s">
         <v>76</v>
       </c>
-      <c r="BW5" t="s">
+      <c r="BX5" t="s">
         <v>101</v>
       </c>
-      <c r="BY5" t="s">
+      <c r="BZ5" t="s">
         <v>116</v>
       </c>
-      <c r="BZ5" t="s">
+      <c r="CA5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>43796</v>
+      </c>
+      <c r="B6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>109</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>110</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>70118</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>118</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>119</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>120</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>88</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>89</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>101</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>121</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>90</v>
       </c>
-      <c r="AB6" t="s">
-        <v>92</v>
-      </c>
       <c r="AC6" t="s">
         <v>92</v>
       </c>
@@ -1788,7 +1807,7 @@
         <v>92</v>
       </c>
       <c r="AE6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AF6" t="s">
         <v>93</v>
@@ -1800,7 +1819,7 @@
         <v>93</v>
       </c>
       <c r="AI6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AJ6" t="s">
         <v>92</v>
@@ -1812,7 +1831,7 @@
         <v>92</v>
       </c>
       <c r="AM6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AN6" t="s">
         <v>95</v>
@@ -1827,11 +1846,11 @@
         <v>95</v>
       </c>
       <c r="AR6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS6" t="s">
         <v>96</v>
       </c>
-      <c r="AS6" t="s">
-        <v>95</v>
-      </c>
       <c r="AT6" t="s">
         <v>95</v>
       </c>
@@ -1842,170 +1861,176 @@
         <v>95</v>
       </c>
       <c r="AW6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AX6" t="s">
         <v>96</v>
       </c>
       <c r="AY6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AZ6" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA6" t="s">
         <v>101</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BB6" t="s">
         <v>122</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BC6" t="s">
         <v>63</v>
       </c>
-      <c r="BD6" t="s">
+      <c r="BE6" t="s">
         <v>65</v>
       </c>
-      <c r="BE6" t="s">
+      <c r="BF6" t="s">
         <v>66</v>
       </c>
-      <c r="BF6" t="s">
+      <c r="BG6" t="s">
         <v>67</v>
       </c>
-      <c r="BG6" t="s">
+      <c r="BH6" t="s">
         <v>68</v>
       </c>
-      <c r="BH6" t="s">
+      <c r="BI6" t="s">
         <v>69</v>
       </c>
-      <c r="BJ6" t="s">
+      <c r="BK6" t="s">
         <v>71</v>
       </c>
-      <c r="BK6" t="s">
+      <c r="BL6" t="s">
         <v>72</v>
       </c>
-      <c r="BO6" t="s">
+      <c r="BP6" t="s">
         <v>75</v>
       </c>
-      <c r="BW6" t="s">
+      <c r="BX6" t="s">
         <v>101</v>
       </c>
-      <c r="BX6" t="s">
+      <c r="BY6" t="s">
         <v>123</v>
       </c>
-      <c r="BY6" t="s">
+      <c r="BZ6" t="s">
         <v>124</v>
       </c>
-      <c r="BZ6" t="s">
+      <c r="CA6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>43795</v>
+      </c>
+      <c r="B7" t="s">
         <v>82</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>109</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>84</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>70118</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>85</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>86</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>2</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>126</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>88</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>89</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>113</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>88</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>89</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>43788</v>
+      </c>
+      <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>84</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>3</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>70118</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>127</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>112</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>2</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>128</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>88</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>89</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>129</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>88</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>89</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>90</v>
       </c>
-      <c r="AB8" t="s">
-        <v>92</v>
-      </c>
       <c r="AC8" t="s">
         <v>92</v>
       </c>
       <c r="AD8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF8" t="s">
         <v>92</v>
@@ -2023,19 +2048,19 @@
         <v>92</v>
       </c>
       <c r="AK8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL8" t="s">
         <v>130</v>
       </c>
-      <c r="AL8" t="s">
-        <v>92</v>
-      </c>
       <c r="AM8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AN8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AO8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AP8" t="s">
         <v>95</v>
@@ -2044,7 +2069,7 @@
         <v>95</v>
       </c>
       <c r="AR8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AS8" t="s">
         <v>97</v>
@@ -2053,135 +2078,138 @@
         <v>97</v>
       </c>
       <c r="AU8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AV8" t="s">
         <v>94</v>
       </c>
-      <c r="AV8" t="s">
-        <v>95</v>
-      </c>
       <c r="AW8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX8" t="s">
         <v>96</v>
       </c>
-      <c r="AX8" t="s">
-        <v>97</v>
-      </c>
       <c r="AY8" t="s">
         <v>97</v>
       </c>
       <c r="AZ8" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA8" t="s">
         <v>101</v>
       </c>
-      <c r="BA8" t="s">
+      <c r="BB8" t="s">
         <v>131</v>
       </c>
-      <c r="BD8" t="s">
+      <c r="BE8" t="s">
         <v>65</v>
       </c>
-      <c r="BE8" t="s">
+      <c r="BF8" t="s">
         <v>66</v>
       </c>
-      <c r="BI8" t="s">
+      <c r="BJ8" t="s">
         <v>70</v>
       </c>
-      <c r="BJ8" t="s">
+      <c r="BK8" t="s">
         <v>71</v>
       </c>
-      <c r="BM8" t="s">
+      <c r="BN8" t="s">
         <v>132</v>
       </c>
-      <c r="BO8" t="s">
+      <c r="BP8" t="s">
         <v>75</v>
       </c>
-      <c r="BW8" t="s">
+      <c r="BX8" t="s">
         <v>101</v>
       </c>
-      <c r="BY8" t="s">
+      <c r="BZ8" t="s">
         <v>133</v>
       </c>
-      <c r="BZ8" t="s">
+      <c r="CA8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>43776.503946759258</v>
+      </c>
+      <c r="B9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>110</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>104</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>70092</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>135</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>136</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>120</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>88</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>137</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="Z9" t="s">
         <v>90</v>
       </c>
-      <c r="AB9" t="s">
-        <v>93</v>
-      </c>
       <c r="AC9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AD9" t="s">
         <v>92</v>
       </c>
       <c r="AE9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AF9" t="s">
         <v>93</v>
       </c>
       <c r="AG9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AH9" t="s">
         <v>92</v>
       </c>
       <c r="AI9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ9" t="s">
         <v>91</v>
       </c>
-      <c r="AJ9" t="s">
-        <v>92</v>
-      </c>
       <c r="AK9" t="s">
         <v>92</v>
       </c>
       <c r="AL9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AN9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AO9" t="s">
         <v>95</v>
@@ -2193,106 +2221,109 @@
         <v>95</v>
       </c>
       <c r="AR9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AS9" t="s">
         <v>94</v>
       </c>
       <c r="AT9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AU9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AV9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AW9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX9" t="s">
         <v>94</v>
       </c>
-      <c r="AX9" t="s">
-        <v>97</v>
-      </c>
       <c r="AY9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AZ9" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA9" t="s">
         <v>101</v>
       </c>
-      <c r="BA9" t="s">
+      <c r="BB9" t="s">
         <v>138</v>
       </c>
-      <c r="BC9" t="s">
+      <c r="BD9" t="s">
         <v>64</v>
       </c>
-      <c r="BE9" t="s">
+      <c r="BF9" t="s">
         <v>66</v>
       </c>
-      <c r="BL9" t="s">
+      <c r="BM9" t="s">
         <v>139</v>
       </c>
-      <c r="BM9" t="s">
+      <c r="BN9" t="s">
         <v>140</v>
       </c>
-      <c r="BO9" t="s">
+      <c r="BP9" t="s">
         <v>75</v>
       </c>
-      <c r="BW9" t="s">
+      <c r="BX9" t="s">
         <v>101</v>
       </c>
-      <c r="BY9" t="s">
+      <c r="BZ9" t="s">
         <v>141</v>
       </c>
-      <c r="BZ9" t="s">
+      <c r="CA9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>43775.374432870369</v>
+      </c>
+      <c r="B10" t="s">
         <v>82</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>109</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>110</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>70119</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>127</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>112</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>1</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>120</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>88</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>37</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>143</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>90</v>
       </c>
-      <c r="AB10" t="s">
-        <v>93</v>
-      </c>
       <c r="AC10" t="s">
         <v>93</v>
       </c>
@@ -2303,7 +2334,7 @@
         <v>93</v>
       </c>
       <c r="AF10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AG10" t="s">
         <v>92</v>
@@ -2318,14 +2349,14 @@
         <v>92</v>
       </c>
       <c r="AK10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL10" t="s">
         <v>130</v>
       </c>
-      <c r="AL10" t="s">
+      <c r="AM10" t="s">
         <v>91</v>
       </c>
-      <c r="AM10" t="s">
-        <v>95</v>
-      </c>
       <c r="AN10" t="s">
         <v>95</v>
       </c>
@@ -2339,13 +2370,13 @@
         <v>95</v>
       </c>
       <c r="AR10" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS10" t="s">
         <v>94</v>
       </c>
-      <c r="AS10" t="s">
-        <v>97</v>
-      </c>
       <c r="AT10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU10" t="s">
         <v>95</v>
@@ -2354,97 +2385,100 @@
         <v>95</v>
       </c>
       <c r="AW10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AX10" t="s">
         <v>96</v>
       </c>
       <c r="AY10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AZ10" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA10" t="s">
         <v>101</v>
       </c>
-      <c r="BA10" t="s">
+      <c r="BB10" t="s">
         <v>144</v>
       </c>
-      <c r="BB10" t="s">
+      <c r="BC10" t="s">
         <v>63</v>
       </c>
-      <c r="BD10" t="s">
+      <c r="BE10" t="s">
         <v>65</v>
       </c>
-      <c r="BE10" t="s">
+      <c r="BF10" t="s">
         <v>66</v>
       </c>
-      <c r="BF10" t="s">
+      <c r="BG10" t="s">
         <v>67</v>
       </c>
-      <c r="BG10" t="s">
+      <c r="BH10" t="s">
         <v>68</v>
       </c>
-      <c r="BJ10" t="s">
+      <c r="BK10" t="s">
         <v>71</v>
       </c>
-      <c r="BS10" t="s">
+      <c r="BT10" t="s">
         <v>79</v>
       </c>
-      <c r="BW10" t="s">
+      <c r="BX10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>43762.409861111111</v>
+      </c>
+      <c r="B11" t="s">
         <v>82</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>109</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>84</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
       </c>
       <c r="F11">
         <v>2</v>
       </c>
       <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
         <v>70117</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>135</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>105</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>2</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>128</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>88</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>89</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>120</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>82</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Y11" t="s">
         <v>89</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Z11" t="s">
         <v>90</v>
       </c>
-      <c r="AB11" t="s">
-        <v>93</v>
-      </c>
       <c r="AC11" t="s">
         <v>93</v>
       </c>
@@ -2476,7 +2510,7 @@
         <v>93</v>
       </c>
       <c r="AM11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN11" t="s">
         <v>95</v>
@@ -2491,13 +2525,13 @@
         <v>95</v>
       </c>
       <c r="AR11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AS11" t="s">
         <v>96</v>
       </c>
       <c r="AT11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AU11" t="s">
         <v>95</v>
@@ -2509,97 +2543,100 @@
         <v>95</v>
       </c>
       <c r="AX11" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY11" t="s">
         <v>96</v>
       </c>
-      <c r="AY11" t="s">
-        <v>95</v>
-      </c>
       <c r="AZ11" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA11" t="s">
         <v>90</v>
       </c>
-      <c r="BC11" t="s">
+      <c r="BD11" t="s">
         <v>64</v>
       </c>
-      <c r="BF11" t="s">
+      <c r="BG11" t="s">
         <v>67</v>
       </c>
-      <c r="BH11" t="s">
+      <c r="BI11" t="s">
         <v>69</v>
       </c>
-      <c r="BJ11" t="s">
+      <c r="BK11" t="s">
         <v>71</v>
       </c>
-      <c r="BS11" t="s">
+      <c r="BT11" t="s">
         <v>79</v>
       </c>
-      <c r="BW11" t="s">
+      <c r="BX11" t="s">
         <v>101</v>
       </c>
-      <c r="BY11" t="s">
+      <c r="BZ11" t="s">
         <v>145</v>
       </c>
-      <c r="BZ11" t="s">
+      <c r="CA11" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>43762.407175925924</v>
+      </c>
+      <c r="B12" t="s">
         <v>82</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>83</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>147</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>2</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>70119</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>148</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>119</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>1</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>113</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>88</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>89</v>
       </c>
-      <c r="Y12" t="s">
+      <c r="Z12" t="s">
         <v>90</v>
       </c>
-      <c r="AB12" t="s">
-        <v>92</v>
-      </c>
       <c r="AC12" t="s">
         <v>92</v>
       </c>
       <c r="AD12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE12" t="s">
         <v>93</v>
       </c>
       <c r="AF12" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG12" t="s">
         <v>91</v>
       </c>
-      <c r="AG12" t="s">
-        <v>92</v>
-      </c>
       <c r="AH12" t="s">
         <v>92</v>
       </c>
@@ -2610,13 +2647,13 @@
         <v>92</v>
       </c>
       <c r="AK12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL12" t="s">
         <v>149</v>
       </c>
-      <c r="AL12" t="s">
-        <v>93</v>
-      </c>
       <c r="AM12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN12" t="s">
         <v>95</v>
@@ -2631,11 +2668,11 @@
         <v>95</v>
       </c>
       <c r="AR12" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS12" t="s">
         <v>94</v>
       </c>
-      <c r="AS12" t="s">
-        <v>95</v>
-      </c>
       <c r="AT12" t="s">
         <v>95</v>
       </c>
@@ -2643,82 +2680,85 @@
         <v>95</v>
       </c>
       <c r="AV12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AW12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AX12" t="s">
         <v>96</v>
       </c>
       <c r="AY12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AZ12" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA12" t="s">
         <v>90</v>
       </c>
-      <c r="BD12" t="s">
+      <c r="BE12" t="s">
         <v>65</v>
       </c>
-      <c r="BJ12" t="s">
+      <c r="BK12" t="s">
         <v>71</v>
       </c>
-      <c r="BV12" t="s">
+      <c r="BW12" t="s">
         <v>150</v>
       </c>
-      <c r="BW12" t="s">
+      <c r="BX12" t="s">
         <v>101</v>
       </c>
-      <c r="BY12" t="s">
+      <c r="BZ12" t="s">
         <v>151</v>
       </c>
-      <c r="BZ12" t="s">
+      <c r="CA12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>43760</v>
+      </c>
+      <c r="B13" t="s">
         <v>82</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>109</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>84</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>3</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>70117</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>85</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>86</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>1</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>87</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>88</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>89</v>
       </c>
-      <c r="Y13" t="s">
+      <c r="Z13" t="s">
         <v>90</v>
       </c>
-      <c r="AB13" t="s">
-        <v>93</v>
-      </c>
       <c r="AC13" t="s">
         <v>93</v>
       </c>
@@ -2750,7 +2790,7 @@
         <v>93</v>
       </c>
       <c r="AM13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN13" t="s">
         <v>95</v>
@@ -2765,16 +2805,16 @@
         <v>95</v>
       </c>
       <c r="AR13" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AS13" t="s">
         <v>94</v>
       </c>
       <c r="AT13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="AU13" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AV13" t="s">
         <v>95</v>
@@ -2783,84 +2823,87 @@
         <v>95</v>
       </c>
       <c r="AX13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY13" t="s">
         <v>96</v>
       </c>
-      <c r="AY13" t="s">
-        <v>95</v>
-      </c>
       <c r="AZ13" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA13" t="s">
         <v>101</v>
       </c>
-      <c r="BH13" t="s">
+      <c r="BI13" t="s">
         <v>69</v>
       </c>
-      <c r="BM13" t="s">
+      <c r="BN13" t="s">
         <v>153</v>
       </c>
-      <c r="BU13" t="s">
+      <c r="BV13" t="s">
         <v>81</v>
       </c>
-      <c r="BW13" t="s">
+      <c r="BX13" t="s">
         <v>101</v>
       </c>
-      <c r="BY13" t="s">
+      <c r="BZ13" t="s">
         <v>154</v>
       </c>
-      <c r="BZ13" t="s">
+      <c r="CA13" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>43749.232719907406</v>
+      </c>
+      <c r="B14" t="s">
         <v>82</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>156</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>84</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>70119</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>157</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>119</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>129</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>88</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>158</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="Z14" t="s">
         <v>90</v>
       </c>
-      <c r="AB14" t="s">
-        <v>93</v>
-      </c>
       <c r="AC14" t="s">
         <v>93</v>
       </c>
       <c r="AD14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AE14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AF14" t="s">
         <v>93</v>
@@ -2878,13 +2921,13 @@
         <v>93</v>
       </c>
       <c r="AK14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AL14" t="s">
         <v>92</v>
       </c>
       <c r="AM14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AN14" t="s">
         <v>95</v>
@@ -2899,16 +2942,16 @@
         <v>95</v>
       </c>
       <c r="AR14" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS14" t="s">
         <v>96</v>
       </c>
-      <c r="AS14" t="s">
-        <v>97</v>
-      </c>
       <c r="AT14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AV14" t="s">
         <v>97</v>
@@ -2923,73 +2966,76 @@
         <v>97</v>
       </c>
       <c r="AZ14" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA14" t="s">
         <v>101</v>
       </c>
-      <c r="BA14" t="s">
+      <c r="BB14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>43748</v>
+      </c>
+      <c r="B15" t="s">
         <v>88</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>109</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>160</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>2</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>3</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>70115</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>157</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>119</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>1</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>128</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>88</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>114</v>
       </c>
-      <c r="Y15" t="s">
+      <c r="Z15" t="s">
         <v>90</v>
       </c>
-      <c r="AB15" t="s">
-        <v>93</v>
-      </c>
       <c r="AC15" t="s">
         <v>93</v>
       </c>
       <c r="AD15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AE15" t="s">
         <v>91</v>
       </c>
-      <c r="AE15" t="s">
-        <v>92</v>
-      </c>
       <c r="AF15" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG15" t="s">
         <v>91</v>
       </c>
-      <c r="AG15" t="s">
-        <v>93</v>
-      </c>
       <c r="AH15" t="s">
         <v>93</v>
       </c>
@@ -3000,13 +3046,13 @@
         <v>93</v>
       </c>
       <c r="AK15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL15" t="s">
         <v>91</v>
       </c>
-      <c r="AL15" t="s">
-        <v>93</v>
-      </c>
       <c r="AM15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN15" t="s">
         <v>95</v>
@@ -3018,17 +3064,17 @@
         <v>95</v>
       </c>
       <c r="AQ15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AR15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS15" t="s">
         <v>96</v>
       </c>
-      <c r="AS15" t="s">
+      <c r="AT15" t="s">
         <v>94</v>
       </c>
-      <c r="AT15" t="s">
-        <v>95</v>
-      </c>
       <c r="AU15" t="s">
         <v>95</v>
       </c>
@@ -3036,76 +3082,79 @@
         <v>95</v>
       </c>
       <c r="AW15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AX15" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY15" t="s">
         <v>94</v>
       </c>
-      <c r="AY15" t="s">
-        <v>95</v>
-      </c>
       <c r="AZ15" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA15" t="s">
         <v>90</v>
       </c>
-      <c r="BP15" t="s">
+      <c r="BQ15" t="s">
         <v>76</v>
       </c>
-      <c r="BW15" t="s">
+      <c r="BX15" t="s">
         <v>101</v>
       </c>
-      <c r="BY15" t="s">
+      <c r="BZ15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>43740.354398148149</v>
+      </c>
+      <c r="B16" t="s">
         <v>82</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>109</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>110</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
       <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
         <v>70124</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>111</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>119</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>1</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>126</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>82</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>89</v>
       </c>
-      <c r="Y16" t="s">
+      <c r="Z16" t="s">
         <v>101</v>
       </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>121</v>
       </c>
-      <c r="AA16" t="s">
+      <c r="AB16" t="s">
         <v>90</v>
       </c>
-      <c r="AB16" t="s">
-        <v>93</v>
-      </c>
       <c r="AC16" t="s">
         <v>93</v>
       </c>
@@ -3137,7 +3186,7 @@
         <v>93</v>
       </c>
       <c r="AM16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN16" t="s">
         <v>95</v>
@@ -3152,13 +3201,13 @@
         <v>95</v>
       </c>
       <c r="AR16" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS16" t="s">
         <v>94</v>
       </c>
-      <c r="AS16" t="s">
-        <v>97</v>
-      </c>
       <c r="AT16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU16" t="s">
         <v>95</v>
@@ -3167,87 +3216,90 @@
         <v>95</v>
       </c>
       <c r="AW16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AX16" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY16" t="s">
         <v>94</v>
       </c>
-      <c r="AY16" t="s">
-        <v>95</v>
-      </c>
       <c r="AZ16" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA16" t="s">
         <v>90</v>
       </c>
-      <c r="BC16" t="s">
+      <c r="BD16" t="s">
         <v>64</v>
       </c>
-      <c r="BM16" t="s">
+      <c r="BN16" t="s">
         <v>162</v>
       </c>
-      <c r="BO16" t="s">
+      <c r="BP16" t="s">
         <v>75</v>
       </c>
-      <c r="BW16" t="s">
+      <c r="BX16" t="s">
         <v>101</v>
       </c>
-      <c r="BY16" t="s">
+      <c r="BZ16" t="s">
         <v>163</v>
       </c>
-      <c r="BZ16" t="s">
+      <c r="CA16" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>43739.537731481483</v>
+      </c>
+      <c r="B17" t="s">
         <v>82</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>109</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>110</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>2</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>3</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>70119</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>111</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>112</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>1</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>113</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>88</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>89</v>
       </c>
-      <c r="Y17" t="s">
+      <c r="Z17" t="s">
         <v>90</v>
       </c>
-      <c r="AB17" t="s">
-        <v>93</v>
-      </c>
       <c r="AC17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AD17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE17" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF17" t="s">
         <v>92</v>
@@ -3265,13 +3317,13 @@
         <v>92</v>
       </c>
       <c r="AK17" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL17" t="s">
         <v>91</v>
       </c>
-      <c r="AL17" t="s">
-        <v>92</v>
-      </c>
       <c r="AM17" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="AN17" t="s">
         <v>95</v>
@@ -3286,13 +3338,13 @@
         <v>95</v>
       </c>
       <c r="AR17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS17" t="s">
         <v>94</v>
       </c>
-      <c r="AS17" t="s">
-        <v>97</v>
-      </c>
       <c r="AT17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU17" t="s">
         <v>95</v>
@@ -3301,102 +3353,105 @@
         <v>95</v>
       </c>
       <c r="AW17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX17" t="s">
         <v>96</v>
       </c>
-      <c r="AX17" t="s">
+      <c r="AY17" t="s">
         <v>94</v>
       </c>
-      <c r="AY17" t="s">
-        <v>97</v>
-      </c>
       <c r="AZ17" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA17" t="s">
         <v>101</v>
       </c>
-      <c r="BA17" t="s">
+      <c r="BB17" t="s">
         <v>165</v>
       </c>
-      <c r="BC17" t="s">
+      <c r="BD17" t="s">
         <v>64</v>
       </c>
-      <c r="BD17" t="s">
+      <c r="BE17" t="s">
         <v>65</v>
       </c>
-      <c r="BE17" t="s">
+      <c r="BF17" t="s">
         <v>66</v>
       </c>
-      <c r="BG17" t="s">
+      <c r="BH17" t="s">
         <v>68</v>
       </c>
-      <c r="BJ17" t="s">
+      <c r="BK17" t="s">
         <v>71</v>
       </c>
-      <c r="BM17" t="s">
+      <c r="BN17" t="s">
         <v>166</v>
       </c>
-      <c r="BO17" t="s">
+      <c r="BP17" t="s">
         <v>75</v>
       </c>
-      <c r="BW17" t="s">
+      <c r="BX17" t="s">
         <v>101</v>
       </c>
-      <c r="BY17" t="s">
+      <c r="BZ17" t="s">
         <v>167</v>
       </c>
-      <c r="BZ17" t="s">
+      <c r="CA17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>43725.755115740743</v>
+      </c>
+      <c r="B18" t="s">
         <v>82</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>168</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>84</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>2</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>70115</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>85</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>136</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>1</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>128</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>82</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>89</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="Z18" t="s">
         <v>90</v>
       </c>
-      <c r="AB18" t="s">
-        <v>93</v>
-      </c>
       <c r="AC18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AD18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF18" t="s">
         <v>92</v>
@@ -3411,19 +3466,19 @@
         <v>92</v>
       </c>
       <c r="AJ18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AK18" t="s">
         <v>93</v>
       </c>
       <c r="AL18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AM18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="AN18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AO18" t="s">
         <v>95</v>
@@ -3432,16 +3487,16 @@
         <v>95</v>
       </c>
       <c r="AQ18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AR18" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS18" t="s">
         <v>94</v>
       </c>
-      <c r="AS18" t="s">
-        <v>97</v>
-      </c>
       <c r="AT18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU18" t="s">
         <v>95</v>
@@ -3450,7 +3505,7 @@
         <v>95</v>
       </c>
       <c r="AW18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AX18" t="s">
         <v>97</v>
@@ -3459,143 +3514,149 @@
         <v>97</v>
       </c>
       <c r="AZ18" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA18" t="s">
         <v>101</v>
       </c>
-      <c r="BA18" t="s">
+      <c r="BB18" t="s">
         <v>169</v>
       </c>
-      <c r="BC18" t="s">
+      <c r="BD18" t="s">
         <v>64</v>
       </c>
-      <c r="BD18" t="s">
+      <c r="BE18" t="s">
         <v>65</v>
       </c>
-      <c r="BH18" t="s">
+      <c r="BI18" t="s">
         <v>69</v>
       </c>
-      <c r="BI18" t="s">
+      <c r="BJ18" t="s">
         <v>70</v>
       </c>
-      <c r="BK18" t="s">
+      <c r="BL18" t="s">
         <v>72</v>
       </c>
-      <c r="BM18" t="s">
+      <c r="BN18" t="s">
         <v>170</v>
       </c>
-      <c r="BS18" t="s">
+      <c r="BT18" t="s">
         <v>79</v>
       </c>
-      <c r="BW18" t="s">
+      <c r="BX18" t="s">
         <v>101</v>
       </c>
-      <c r="BY18" t="s">
+      <c r="BZ18" t="s">
         <v>107</v>
       </c>
-      <c r="BZ18" t="s">
+      <c r="CA18" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="19" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>43720.744293981479</v>
+      </c>
+      <c r="B19" t="s">
         <v>82</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>110</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>2</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>1</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>70119</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>127</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>119</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>1</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>87</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>88</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>89</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>101</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AA19" t="s">
         <v>121</v>
       </c>
-      <c r="AA19" t="s">
+      <c r="AB19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>43719.629212962966</v>
+      </c>
+      <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>110</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>2</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>1</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>70119</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>85</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>86</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>1</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>87</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>82</v>
       </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>89</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="Z20" t="s">
         <v>90</v>
       </c>
-      <c r="AB20" t="s">
-        <v>93</v>
-      </c>
       <c r="AC20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AD20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AE20" t="s">
         <v>93</v>
       </c>
       <c r="AF20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AG20" t="s">
         <v>92</v>
@@ -3604,22 +3665,22 @@
         <v>92</v>
       </c>
       <c r="AI20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AJ20" t="s">
         <v>93</v>
       </c>
       <c r="AK20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL20" t="s">
         <v>149</v>
       </c>
-      <c r="AL20" t="s">
-        <v>93</v>
-      </c>
       <c r="AM20" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AN20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AO20" t="s">
         <v>95</v>
@@ -3628,147 +3689,150 @@
         <v>95</v>
       </c>
       <c r="AQ20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AR20" t="s">
+        <v>97</v>
+      </c>
+      <c r="AS20" t="s">
         <v>94</v>
       </c>
-      <c r="AS20" t="s">
-        <v>97</v>
-      </c>
       <c r="AT20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AV20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AW20" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX20" t="s">
         <v>96</v>
       </c>
-      <c r="AX20" t="s">
+      <c r="AY20" t="s">
         <v>94</v>
       </c>
-      <c r="AY20" t="s">
-        <v>95</v>
-      </c>
       <c r="AZ20" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA20" t="s">
         <v>101</v>
       </c>
-      <c r="BA20" t="s">
+      <c r="BB20" t="s">
         <v>172</v>
       </c>
-      <c r="BC20" t="s">
+      <c r="BD20" t="s">
         <v>64</v>
       </c>
-      <c r="BE20" t="s">
+      <c r="BF20" t="s">
         <v>66</v>
       </c>
-      <c r="BM20" t="s">
+      <c r="BN20" t="s">
         <v>173</v>
       </c>
-      <c r="BO20" t="s">
+      <c r="BP20" t="s">
         <v>75</v>
       </c>
-      <c r="BW20" t="s">
+      <c r="BX20" t="s">
         <v>101</v>
       </c>
-      <c r="BY20" t="s">
+      <c r="BZ20" t="s">
         <v>174</v>
       </c>
-      <c r="BZ20" t="s">
+      <c r="CA20" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>43718.555925925924</v>
+      </c>
+      <c r="B21" t="s">
         <v>82</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>83</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>110</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>3</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>70119</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>85</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>136</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>2</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>113</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>88</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>89</v>
       </c>
-      <c r="U21" t="s">
+      <c r="V21" t="s">
         <v>129</v>
       </c>
-      <c r="V21" t="s">
+      <c r="W21" t="s">
         <v>82</v>
       </c>
-      <c r="X21" t="s">
+      <c r="Y21" t="s">
         <v>89</v>
       </c>
-      <c r="Y21" t="s">
+      <c r="Z21" t="s">
         <v>90</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AC21" t="s">
         <v>91</v>
       </c>
-      <c r="AC21" t="s">
-        <v>92</v>
-      </c>
       <c r="AD21" t="s">
         <v>92</v>
       </c>
       <c r="AE21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF21" t="s">
         <v>91</v>
       </c>
-      <c r="AF21" t="s">
-        <v>92</v>
-      </c>
       <c r="AG21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH21" t="s">
         <v>91</v>
       </c>
-      <c r="AH21" t="s">
-        <v>92</v>
-      </c>
       <c r="AI21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AJ21" t="s">
         <v>91</v>
       </c>
       <c r="AK21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AL21" t="s">
         <v>92</v>
       </c>
       <c r="AM21" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="AN21" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AO21" t="s">
         <v>95</v>
@@ -3777,13 +3841,13 @@
         <v>95</v>
       </c>
       <c r="AQ21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AR21" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AS21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AT21" t="s">
         <v>97</v>
@@ -3795,61 +3859,64 @@
         <v>97</v>
       </c>
       <c r="AW21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AX21" t="s">
         <v>96</v>
       </c>
-      <c r="AX21" t="s">
-        <v>97</v>
-      </c>
       <c r="AY21" t="s">
         <v>97</v>
       </c>
       <c r="AZ21" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>43718.542303240742</v>
+      </c>
+      <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>83</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>110</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
         <v>70124</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>127</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>86</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>1</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>87</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>88</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>89</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>90</v>
       </c>
-      <c r="AB22" t="s">
-        <v>93</v>
-      </c>
       <c r="AC22" t="s">
         <v>93</v>
       </c>
@@ -3857,7 +3924,7 @@
         <v>93</v>
       </c>
       <c r="AE22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AF22" t="s">
         <v>92</v>
@@ -3866,7 +3933,7 @@
         <v>92</v>
       </c>
       <c r="AH22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AI22" t="s">
         <v>93</v>
@@ -3875,13 +3942,13 @@
         <v>93</v>
       </c>
       <c r="AK22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AL22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AM22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AN22" t="s">
         <v>95</v>
@@ -3896,95 +3963,101 @@
         <v>95</v>
       </c>
       <c r="AR22" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS22" t="s">
         <v>96</v>
       </c>
-      <c r="AS22" t="s">
-        <v>97</v>
-      </c>
       <c r="AT22" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AU22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AV22" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AW22" t="s">
+        <v>95</v>
+      </c>
+      <c r="AX22" t="s">
         <v>96</v>
       </c>
-      <c r="AX22" t="s">
+      <c r="AY22" t="s">
         <v>94</v>
       </c>
-      <c r="AY22" t="s">
-        <v>97</v>
-      </c>
       <c r="AZ22" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA22" t="s">
         <v>101</v>
       </c>
-      <c r="BA22" t="s">
+      <c r="BB22" t="s">
         <v>176</v>
       </c>
-      <c r="BB22" t="s">
+      <c r="BC22" t="s">
         <v>63</v>
       </c>
-      <c r="BK22" t="s">
+      <c r="BL22" t="s">
         <v>72</v>
       </c>
-      <c r="BM22" t="s">
+      <c r="BN22" t="s">
         <v>177</v>
       </c>
-      <c r="BR22" t="s">
+      <c r="BS22" t="s">
         <v>78</v>
       </c>
-      <c r="BW22" t="s">
+      <c r="BX22" t="s">
         <v>101</v>
       </c>
-      <c r="BY22" t="s">
+      <c r="BZ22" t="s">
         <v>178</v>
       </c>
-      <c r="BZ22" t="s">
+      <c r="CA22" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:78" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>43706.742766203701</v>
+      </c>
+      <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>180</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>84</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="G23">
-        <v>70119</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>70119</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23">
+        <v>70119</v>
+      </c>
+      <c r="J23" t="s">
         <v>135</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>105</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>1</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>87</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>88</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>181</v>
       </c>
     </row>

</xml_diff>